<commit_message>
added verschnitt and returns
</commit_message>
<xml_diff>
--- a/Produktionsplanung.xlsx
+++ b/Produktionsplanung.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacob/development/OperationsResearch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254C4C57-3606-D541-AF91-64FDFF3965CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A479FB85-1B7F-E44A-AA44-376FAC07F365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produkt" sheetId="1" r:id="rId1"/>
     <sheet name="Material" sheetId="2" r:id="rId2"/>
     <sheet name="Fixkosten" sheetId="3" r:id="rId3"/>
+    <sheet name="Variablen" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
   <si>
     <t>1. Material - Beschreibung</t>
   </si>
@@ -140,6 +141,18 @@
   </si>
   <si>
     <t>Modeschau</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Wert</t>
+  </si>
+  <si>
+    <t>Rücksendekosten</t>
+  </si>
+  <si>
+    <t>0.1</t>
   </si>
 </sst>
 </file>
@@ -503,7 +516,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView zoomScale="116" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -947,7 +960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55978B38-B140-6641-A8C9-1B071436B0E7}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -986,13 +999,45 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552D7A01-3CD9-4843-9EB8-8AC2EBDD22C7}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1134,15 +1179,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEC03C23-D6E8-4139-81CC-07BD05490AB4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8282A036-8EF6-43C3-9A77-E061937AACA0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="b124e3ab-2c59-43c0-bd7b-ba8f7c2d92b3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1166,17 +1222,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8282A036-8EF6-43C3-9A77-E061937AACA0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEC03C23-D6E8-4139-81CC-07BD05490AB4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="b124e3ab-2c59-43c0-bd7b-ba8f7c2d92b3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added new File to calculate c)
</commit_message>
<xml_diff>
--- a/Produktionsplanung.xlsx
+++ b/Produktionsplanung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacob/development/OperationsResearch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E3512E-8632-DC4D-8F41-76D45DAC6CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6893F11E-2AE4-3947-AFAD-ECB61E42F523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produkt" sheetId="1" r:id="rId1"/>
@@ -512,7 +512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="116" workbookViewId="0">
+    <sheetView zoomScale="116" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -806,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B6EE40-1C94-2E48-BE0A-BB4D5DDD6BD4}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -990,21 +990,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100AED214031F7E024FB76640D948FD5950" ma:contentTypeVersion="3" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="5304f045f5abf8a2a6fd79f3cf7a33b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b124e3ab-2c59-43c0-bd7b-ba8f7c2d92b3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b005e430761d8441af683b9762c19bae" ns2:_="">
     <xsd:import namespace="b124e3ab-2c59-43c0-bd7b-ba8f7c2d92b3"/>
@@ -1142,31 +1127,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8282A036-8EF6-43C3-9A77-E061937AACA0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="b124e3ab-2c59-43c0-bd7b-ba8f7c2d92b3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEC03C23-D6E8-4139-81CC-07BD05490AB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E07A43E1-E761-4DD7-9F75-67699012D606}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1182,4 +1158,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEC03C23-D6E8-4139-81CC-07BD05490AB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8282A036-8EF6-43C3-9A77-E061937AACA0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="b124e3ab-2c59-43c0-bd7b-ba8f7c2d92b3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>